<commit_message>
adicionado o gustavo e alterado a liliane e excluido o mauricio
</commit_message>
<xml_diff>
--- a/public/assets/planilha_de_ramais.xlsx
+++ b/public/assets/planilha_de_ramais.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafael.almeida\Desktop\ramais\lista-de-ramais\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E58B4C9-8534-49E6-9D7B-B63D5566A84E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDDB587C-CA57-4898-9D93-994C96BD8038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{45DE8AC7-1F08-4348-9830-FFE096CC0B59}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="122">
   <si>
     <t>Ana Villegas</t>
   </si>
@@ -189,12 +189,6 @@
     <t>Liliane Souza</t>
   </si>
   <si>
-    <t>Comercial / Faturamento</t>
-  </si>
-  <si>
-    <t>Assistente Comercial</t>
-  </si>
-  <si>
     <t>liliane.souza@brasmol.com.br</t>
   </si>
   <si>
@@ -216,21 +210,12 @@
     <t>Analista Técnico</t>
   </si>
   <si>
-    <t>Mauricio Araujo</t>
-  </si>
-  <si>
     <t>Compras</t>
   </si>
   <si>
     <t>Comprador</t>
   </si>
   <si>
-    <t>mauricio.araujo@brasmol.com.br</t>
-  </si>
-  <si>
-    <t>https://i.postimg.cc/ZYpvcCpN/Mauricio-Araujo-Figueredo.jpg</t>
-  </si>
-  <si>
     <t>Nordon Jose</t>
   </si>
   <si>
@@ -406,6 +391,18 @@
   </si>
   <si>
     <t>https://i.postimg.cc/dtH1L84q/Janildo-Franco-da-Costa.png</t>
+  </si>
+  <si>
+    <t>Gustavo Onofre</t>
+  </si>
+  <si>
+    <t>gustavo.onofre@brasmol.com.br</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/fb3zX5Wr/54462329-2023386377772706-632683506295635968-n-removebg-preview.png</t>
+  </si>
+  <si>
+    <t>Compradora</t>
   </si>
 </sst>
 </file>
@@ -771,7 +768,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,42 +782,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B1" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C1" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D1" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E1" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B2">
         <v>145</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -905,22 +902,22 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B7">
         <v>117</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D7" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -928,7 +925,7 @@
         <v>24</v>
       </c>
       <c r="B8">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
@@ -1002,144 +999,144 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>118</v>
       </c>
       <c r="B12">
-        <v>154</v>
+        <v>128</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>43</v>
+        <v>119</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>42</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>118</v>
+        <v>39</v>
       </c>
       <c r="B13">
-        <v>120</v>
+        <v>154</v>
       </c>
       <c r="C13" t="s">
-        <v>119</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
-        <v>120</v>
+        <v>41</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>121</v>
+        <v>43</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>122</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>113</v>
       </c>
       <c r="B14">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>114</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>48</v>
+        <v>116</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>47</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B15">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D15" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16">
+        <v>128</v>
+      </c>
+      <c r="C16" t="s">
         <v>57</v>
       </c>
-      <c r="B16">
+      <c r="D16" t="s">
         <v>121</v>
       </c>
-      <c r="C16" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" t="s">
-        <v>58</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B17">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B18">
         <v>111</v>
       </c>
       <c r="C18" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D18" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B19">
         <v>131</v>
@@ -1148,78 +1145,78 @@
         <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B20">
         <v>114</v>
       </c>
       <c r="C20" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B21">
         <v>135</v>
       </c>
       <c r="C21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" t="s">
         <v>56</v>
       </c>
-      <c r="D21" t="s">
-        <v>58</v>
-      </c>
       <c r="E21" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B22">
         <v>117</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D22" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B23">
         <v>118</v>
@@ -1228,38 +1225,38 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B24">
         <v>139</v>
       </c>
       <c r="C24" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D24" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B25">
         <v>147</v>
@@ -1268,64 +1265,64 @@
         <v>35</v>
       </c>
       <c r="D25" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B26">
         <v>130</v>
       </c>
       <c r="C26" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B27">
         <v>111</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D27" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B28">
         <v>145</v>
       </c>
       <c r="C28" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D28" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1350,41 +1347,41 @@
     <hyperlink ref="F10" r:id="rId13" xr:uid="{E09195E1-1C24-462C-B879-81B1F2B2AD46}"/>
     <hyperlink ref="F11" r:id="rId14" xr:uid="{1C19DA5E-F4EC-4AB5-82A6-F6324DA88C6F}"/>
     <hyperlink ref="E11" r:id="rId15" xr:uid="{A902CE3A-637E-4997-B213-59454CD24F00}"/>
-    <hyperlink ref="F12" r:id="rId16" xr:uid="{F4B32BFF-7F63-4A5E-BB74-3804F7009221}"/>
-    <hyperlink ref="E12" r:id="rId17" xr:uid="{3F9C83B9-6D79-422D-B2AB-F82F425D6A1A}"/>
-    <hyperlink ref="F14" r:id="rId18" xr:uid="{1E5A1A7D-10CB-4A69-B3B7-5A96A58852E8}"/>
-    <hyperlink ref="E14" r:id="rId19" xr:uid="{2A1437AD-EB64-4D57-93DA-B8505C0A089D}"/>
-    <hyperlink ref="E15" r:id="rId20" xr:uid="{8C043714-3FA3-4036-9689-001EB3D08E5F}"/>
-    <hyperlink ref="F15" r:id="rId21" xr:uid="{1CBF6B7D-F8CC-414D-A08D-963F86FCF154}"/>
-    <hyperlink ref="F16" r:id="rId22" xr:uid="{DB962BA9-C20F-4D9C-9E3F-5B8FB8DB9C50}"/>
-    <hyperlink ref="E16" r:id="rId23" xr:uid="{56E1324E-1283-4C86-88C5-39D7C2E7E18E}"/>
-    <hyperlink ref="E17" r:id="rId24" xr:uid="{BABD07CA-AAE5-47FB-A114-CEDA897A3791}"/>
-    <hyperlink ref="F17" r:id="rId25" xr:uid="{A1DB2D97-442B-4024-83A5-DF60597BF134}"/>
-    <hyperlink ref="E19" r:id="rId26" xr:uid="{6C25687E-59DD-4AD8-8DED-B57E3370F478}"/>
-    <hyperlink ref="F19" r:id="rId27" xr:uid="{5EB6A491-6932-4244-80A6-8932A90C8C2D}"/>
-    <hyperlink ref="E20" r:id="rId28" xr:uid="{33C62798-3902-4381-AF7F-D52EA1735BDF}"/>
-    <hyperlink ref="F20" r:id="rId29" xr:uid="{5402F469-AAA0-47CE-98A3-3A3702BE2533}"/>
-    <hyperlink ref="E21" r:id="rId30" xr:uid="{F7001A1F-E6A6-4FF7-8229-1768BC34202A}"/>
-    <hyperlink ref="F21" r:id="rId31" xr:uid="{0E37CBC2-3F46-4C7D-BFCE-BA161B82EEEF}"/>
-    <hyperlink ref="E22" r:id="rId32" xr:uid="{3A614AC7-A418-4D05-9D6E-131F8051C85C}"/>
-    <hyperlink ref="F22" r:id="rId33" xr:uid="{305353EA-88E1-411A-AAED-D15872793A1B}"/>
-    <hyperlink ref="E23" r:id="rId34" xr:uid="{47750F49-BBBA-426E-9AEB-FAA74663AA50}"/>
-    <hyperlink ref="F23" r:id="rId35" xr:uid="{88D9947E-3193-40D4-B039-2D20AC904B8B}"/>
-    <hyperlink ref="F27" r:id="rId36" xr:uid="{572392B9-9359-4BD0-88A9-A54028FBA06C}"/>
-    <hyperlink ref="F18" r:id="rId37" xr:uid="{B3BEEF97-5FF4-4685-A32A-0560E55D99BD}"/>
-    <hyperlink ref="E24" r:id="rId38" xr:uid="{9872AE2B-7D2E-48FD-8144-246F095810A8}"/>
-    <hyperlink ref="F24" r:id="rId39" xr:uid="{971C9123-0B1A-44B1-9E93-EBCDB15BB1C3}"/>
-    <hyperlink ref="E25" r:id="rId40" xr:uid="{8FA3B366-19B9-4E84-9CA7-5FA310A37CD2}"/>
-    <hyperlink ref="F25" r:id="rId41" xr:uid="{F74AF90C-8DCA-48BE-A77E-6F7E8469AC4E}"/>
-    <hyperlink ref="E28" r:id="rId42" xr:uid="{B42644BC-A94C-467A-B0E6-611C15657B88}"/>
-    <hyperlink ref="F28" r:id="rId43" xr:uid="{F8B5C0C4-43CA-4BC2-BE06-EDA7909FECD4}"/>
-    <hyperlink ref="F26" r:id="rId44" xr:uid="{59EDB2A5-1A1E-4F75-BD5A-1081A001173D}"/>
-    <hyperlink ref="E2" r:id="rId45" xr:uid="{79578A44-1938-4C7E-988B-EFB98C810BD5}"/>
-    <hyperlink ref="F2" r:id="rId46" xr:uid="{00ECDD57-2540-4FA1-A381-08FF55FA83EF}"/>
-    <hyperlink ref="E7" r:id="rId47" xr:uid="{C114CFCC-6D82-413F-819F-1EDA67E0910A}"/>
-    <hyperlink ref="F7" r:id="rId48" xr:uid="{A484D214-DAC7-4BD3-B31F-0750843CF374}"/>
-    <hyperlink ref="E13" r:id="rId49" xr:uid="{DDA1AF5D-ACDF-433A-8BD3-4D814E2618E0}"/>
-    <hyperlink ref="F13" r:id="rId50" xr:uid="{26F222F3-E8B4-4247-A004-06C0FE1AC086}"/>
+    <hyperlink ref="F13" r:id="rId16" xr:uid="{F4B32BFF-7F63-4A5E-BB74-3804F7009221}"/>
+    <hyperlink ref="E13" r:id="rId17" xr:uid="{3F9C83B9-6D79-422D-B2AB-F82F425D6A1A}"/>
+    <hyperlink ref="F15" r:id="rId18" xr:uid="{1E5A1A7D-10CB-4A69-B3B7-5A96A58852E8}"/>
+    <hyperlink ref="E15" r:id="rId19" xr:uid="{2A1437AD-EB64-4D57-93DA-B8505C0A089D}"/>
+    <hyperlink ref="E16" r:id="rId20" xr:uid="{8C043714-3FA3-4036-9689-001EB3D08E5F}"/>
+    <hyperlink ref="F16" r:id="rId21" xr:uid="{1CBF6B7D-F8CC-414D-A08D-963F86FCF154}"/>
+    <hyperlink ref="F17" r:id="rId22" xr:uid="{DB962BA9-C20F-4D9C-9E3F-5B8FB8DB9C50}"/>
+    <hyperlink ref="E17" r:id="rId23" xr:uid="{56E1324E-1283-4C86-88C5-39D7C2E7E18E}"/>
+    <hyperlink ref="E19" r:id="rId24" xr:uid="{6C25687E-59DD-4AD8-8DED-B57E3370F478}"/>
+    <hyperlink ref="F19" r:id="rId25" xr:uid="{5EB6A491-6932-4244-80A6-8932A90C8C2D}"/>
+    <hyperlink ref="E20" r:id="rId26" xr:uid="{33C62798-3902-4381-AF7F-D52EA1735BDF}"/>
+    <hyperlink ref="F20" r:id="rId27" xr:uid="{5402F469-AAA0-47CE-98A3-3A3702BE2533}"/>
+    <hyperlink ref="E21" r:id="rId28" xr:uid="{F7001A1F-E6A6-4FF7-8229-1768BC34202A}"/>
+    <hyperlink ref="F21" r:id="rId29" xr:uid="{0E37CBC2-3F46-4C7D-BFCE-BA161B82EEEF}"/>
+    <hyperlink ref="E22" r:id="rId30" xr:uid="{3A614AC7-A418-4D05-9D6E-131F8051C85C}"/>
+    <hyperlink ref="F22" r:id="rId31" xr:uid="{305353EA-88E1-411A-AAED-D15872793A1B}"/>
+    <hyperlink ref="E23" r:id="rId32" xr:uid="{47750F49-BBBA-426E-9AEB-FAA74663AA50}"/>
+    <hyperlink ref="F23" r:id="rId33" xr:uid="{88D9947E-3193-40D4-B039-2D20AC904B8B}"/>
+    <hyperlink ref="F27" r:id="rId34" xr:uid="{572392B9-9359-4BD0-88A9-A54028FBA06C}"/>
+    <hyperlink ref="F18" r:id="rId35" xr:uid="{B3BEEF97-5FF4-4685-A32A-0560E55D99BD}"/>
+    <hyperlink ref="E24" r:id="rId36" xr:uid="{9872AE2B-7D2E-48FD-8144-246F095810A8}"/>
+    <hyperlink ref="F24" r:id="rId37" xr:uid="{971C9123-0B1A-44B1-9E93-EBCDB15BB1C3}"/>
+    <hyperlink ref="E25" r:id="rId38" xr:uid="{8FA3B366-19B9-4E84-9CA7-5FA310A37CD2}"/>
+    <hyperlink ref="F25" r:id="rId39" xr:uid="{F74AF90C-8DCA-48BE-A77E-6F7E8469AC4E}"/>
+    <hyperlink ref="E28" r:id="rId40" xr:uid="{B42644BC-A94C-467A-B0E6-611C15657B88}"/>
+    <hyperlink ref="F28" r:id="rId41" xr:uid="{F8B5C0C4-43CA-4BC2-BE06-EDA7909FECD4}"/>
+    <hyperlink ref="F26" r:id="rId42" xr:uid="{59EDB2A5-1A1E-4F75-BD5A-1081A001173D}"/>
+    <hyperlink ref="E2" r:id="rId43" xr:uid="{79578A44-1938-4C7E-988B-EFB98C810BD5}"/>
+    <hyperlink ref="F2" r:id="rId44" xr:uid="{00ECDD57-2540-4FA1-A381-08FF55FA83EF}"/>
+    <hyperlink ref="E7" r:id="rId45" xr:uid="{C114CFCC-6D82-413F-819F-1EDA67E0910A}"/>
+    <hyperlink ref="F7" r:id="rId46" xr:uid="{A484D214-DAC7-4BD3-B31F-0750843CF374}"/>
+    <hyperlink ref="E14" r:id="rId47" xr:uid="{DDA1AF5D-ACDF-433A-8BD3-4D814E2618E0}"/>
+    <hyperlink ref="F14" r:id="rId48" xr:uid="{26F222F3-E8B4-4247-A004-06C0FE1AC086}"/>
+    <hyperlink ref="E12" r:id="rId49" xr:uid="{BD6AB108-0343-4A71-9809-30B5EDCEEC69}"/>
+    <hyperlink ref="F12" r:id="rId50" xr:uid="{B0B85B43-52EE-4D1C-AF35-66EA10DE5D3B}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Removido o Gustavo e adicionada a Elaine
</commit_message>
<xml_diff>
--- a/public/assets/planilha_de_ramais.xlsx
+++ b/public/assets/planilha_de_ramais.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafael.almeida\Desktop\ramais\lista-de-ramais\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDDB587C-CA57-4898-9D93-994C96BD8038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D876E4-9234-4117-B2FB-D2AC0FCC2C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{45DE8AC7-1F08-4348-9830-FFE096CC0B59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{45DE8AC7-1F08-4348-9830-FFE096CC0B59}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$F$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$F$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -213,9 +213,6 @@
     <t>Compras</t>
   </si>
   <si>
-    <t>Comprador</t>
-  </si>
-  <si>
     <t>Nordon Jose</t>
   </si>
   <si>
@@ -393,16 +390,19 @@
     <t>https://i.postimg.cc/dtH1L84q/Janildo-Franco-da-Costa.png</t>
   </si>
   <si>
-    <t>Gustavo Onofre</t>
-  </si>
-  <si>
-    <t>gustavo.onofre@brasmol.com.br</t>
-  </si>
-  <si>
-    <t>https://i.postimg.cc/fb3zX5Wr/54462329-2023386377772706-632683506295635968-n-removebg-preview.png</t>
-  </si>
-  <si>
     <t>Compradora</t>
+  </si>
+  <si>
+    <t>Elaine Alves</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Assistente Comercial </t>
+  </si>
+  <si>
+    <t>elaine.alves@brasmol.com.br</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/wB1VDBHP/file-2.png</t>
   </si>
 </sst>
 </file>
@@ -768,7 +768,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,42 +782,42 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" t="s">
         <v>100</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>101</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>102</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>103</v>
-      </c>
-      <c r="F1" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B2">
         <v>145</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -902,22 +902,22 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B7">
         <v>117</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -942,79 +942,79 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>118</v>
       </c>
       <c r="B9">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>119</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>120</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>19</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B10">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B11">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>118</v>
+        <v>34</v>
       </c>
       <c r="B12">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>119</v>
+        <v>38</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>120</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1039,22 +1039,22 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B14">
         <v>120</v>
       </c>
       <c r="C14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" t="s">
         <v>114</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="F14" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1088,7 +1088,7 @@
         <v>57</v>
       </c>
       <c r="D16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>50</v>
@@ -1119,24 +1119,24 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B18">
         <v>111</v>
       </c>
       <c r="C18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" t="s">
         <v>81</v>
       </c>
-      <c r="D18" t="s">
-        <v>82</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19">
         <v>131</v>
@@ -1145,38 +1145,38 @@
         <v>35</v>
       </c>
       <c r="D19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20">
         <v>114</v>
       </c>
       <c r="C20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" t="s">
         <v>64</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B21">
         <v>135</v>
@@ -1188,35 +1188,35 @@
         <v>56</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22">
         <v>117</v>
       </c>
       <c r="C22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" t="s">
         <v>72</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B23">
         <v>118</v>
@@ -1225,38 +1225,38 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B24">
         <v>139</v>
       </c>
       <c r="C24" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" t="s">
         <v>87</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B25">
         <v>147</v>
@@ -1265,70 +1265,70 @@
         <v>35</v>
       </c>
       <c r="D25" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B26">
         <v>130</v>
       </c>
       <c r="C26" t="s">
+        <v>104</v>
+      </c>
+      <c r="F26" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B27">
         <v>111</v>
       </c>
       <c r="C27" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" t="s">
         <v>81</v>
       </c>
-      <c r="D27" t="s">
+      <c r="F27" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B28">
         <v>145</v>
       </c>
       <c r="C28" t="s">
+        <v>95</v>
+      </c>
+      <c r="D28" t="s">
         <v>96</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>99</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F27" xr:uid="{C900014C-14C8-4838-8849-A03641E53F4B}">
+  <autoFilter ref="A1:F26" xr:uid="{C900014C-14C8-4838-8849-A03641E53F4B}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F28">
-      <sortCondition ref="A1:A27"/>
+      <sortCondition ref="A1:A26"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
@@ -1338,15 +1338,15 @@
     <hyperlink ref="F4" r:id="rId4" xr:uid="{38097E97-2058-4E0E-9D08-A2EABD4C7D54}"/>
     <hyperlink ref="E5" r:id="rId5" xr:uid="{97820ED1-887A-4D19-85CC-BE51457E70B1}"/>
     <hyperlink ref="F5" r:id="rId6" xr:uid="{EDD40362-5662-4ED9-9862-E57C0BFF7BB4}"/>
-    <hyperlink ref="F9" r:id="rId7" xr:uid="{0506CF56-690F-4390-B6C4-241DBEF741D8}"/>
+    <hyperlink ref="F10" r:id="rId7" xr:uid="{0506CF56-690F-4390-B6C4-241DBEF741D8}"/>
     <hyperlink ref="E6" r:id="rId8" xr:uid="{92283AD9-E1E7-4611-B033-7633690F6195}"/>
     <hyperlink ref="F6" r:id="rId9" xr:uid="{C00891E6-9964-4EAE-88A0-073267DB01EB}"/>
     <hyperlink ref="E8" r:id="rId10" xr:uid="{3E5CF3F8-A12D-441E-A7EA-E24ACBAE0D10}"/>
     <hyperlink ref="F8" r:id="rId11" xr:uid="{C2FDF182-A219-48C0-8A97-93DE0A0C1C17}"/>
-    <hyperlink ref="E10" r:id="rId12" xr:uid="{5564ABD7-FC27-479C-9234-BB04AAFDE1CC}"/>
-    <hyperlink ref="F10" r:id="rId13" xr:uid="{E09195E1-1C24-462C-B879-81B1F2B2AD46}"/>
-    <hyperlink ref="F11" r:id="rId14" xr:uid="{1C19DA5E-F4EC-4AB5-82A6-F6324DA88C6F}"/>
-    <hyperlink ref="E11" r:id="rId15" xr:uid="{A902CE3A-637E-4997-B213-59454CD24F00}"/>
+    <hyperlink ref="E11" r:id="rId12" xr:uid="{5564ABD7-FC27-479C-9234-BB04AAFDE1CC}"/>
+    <hyperlink ref="F11" r:id="rId13" xr:uid="{E09195E1-1C24-462C-B879-81B1F2B2AD46}"/>
+    <hyperlink ref="F12" r:id="rId14" xr:uid="{1C19DA5E-F4EC-4AB5-82A6-F6324DA88C6F}"/>
+    <hyperlink ref="E12" r:id="rId15" xr:uid="{A902CE3A-637E-4997-B213-59454CD24F00}"/>
     <hyperlink ref="F13" r:id="rId16" xr:uid="{F4B32BFF-7F63-4A5E-BB74-3804F7009221}"/>
     <hyperlink ref="E13" r:id="rId17" xr:uid="{3F9C83B9-6D79-422D-B2AB-F82F425D6A1A}"/>
     <hyperlink ref="F15" r:id="rId18" xr:uid="{1E5A1A7D-10CB-4A69-B3B7-5A96A58852E8}"/>
@@ -1380,8 +1380,8 @@
     <hyperlink ref="F7" r:id="rId46" xr:uid="{A484D214-DAC7-4BD3-B31F-0750843CF374}"/>
     <hyperlink ref="E14" r:id="rId47" xr:uid="{DDA1AF5D-ACDF-433A-8BD3-4D814E2618E0}"/>
     <hyperlink ref="F14" r:id="rId48" xr:uid="{26F222F3-E8B4-4247-A004-06C0FE1AC086}"/>
-    <hyperlink ref="E12" r:id="rId49" xr:uid="{BD6AB108-0343-4A71-9809-30B5EDCEEC69}"/>
-    <hyperlink ref="F12" r:id="rId50" xr:uid="{B0B85B43-52EE-4D1C-AF35-66EA10DE5D3B}"/>
+    <hyperlink ref="E9" r:id="rId49" xr:uid="{91A7B212-F61A-4001-8B0E-4D95918FCF47}"/>
+    <hyperlink ref="F9" r:id="rId50" xr:uid="{487A1BAA-2AB3-44FE-B188-20C6D73F4F34}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajustes no layout e adição de descrições
</commit_message>
<xml_diff>
--- a/public/assets/planilha_de_ramais.xlsx
+++ b/public/assets/planilha_de_ramais.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rafael.almeida\Desktop\ramais\lista-de-ramais\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E0BC1D1-B214-48F1-AC00-28B679098213}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C1F545-5898-4660-BB0A-E992A9D717DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{45DE8AC7-1F08-4348-9830-FFE096CC0B59}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="131">
   <si>
     <t>Ana Villegas</t>
   </si>
@@ -63,9 +63,6 @@
     <t xml:space="preserve">Gestão da Qualidade </t>
   </si>
   <si>
-    <t>Supervisor da Gestão da Qualidade</t>
-  </si>
-  <si>
     <t>anderson.goveia@brasmol.com.br</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t>Cozinha / Limpeza</t>
   </si>
   <si>
-    <t>Auxiliar e Serviços Gerais</t>
-  </si>
-  <si>
     <t>https://i.postimg.cc/ydTP2k9L/Filomena-Martins-Pereira.jpg</t>
   </si>
   <si>
@@ -207,9 +201,6 @@
     <t>Marcio Mario</t>
   </si>
   <si>
-    <t>Analista Técnico</t>
-  </si>
-  <si>
     <t>Compras</t>
   </si>
   <si>
@@ -327,9 +318,6 @@
     <t>Controle de Qualidade</t>
   </si>
   <si>
-    <t>Inspetor de Qualidade</t>
-  </si>
-  <si>
     <t>controle@brasmol.com.br</t>
   </si>
   <si>
@@ -363,9 +351,6 @@
     <t xml:space="preserve">	Aiume Freitas</t>
   </si>
   <si>
-    <t>Auxiliar de Produção</t>
-  </si>
-  <si>
     <t>https://i.postimg.cc/B6qN79Dc/Aiume-Freitas-Ferreira.png</t>
   </si>
   <si>
@@ -381,9 +366,6 @@
     <t>Projetista de Ferramentas</t>
   </si>
   <si>
-    <t>Compradora</t>
-  </si>
-  <si>
     <t>Elaine Alves</t>
   </si>
   <si>
@@ -400,13 +382,69 @@
   </si>
   <si>
     <t>eduardo.mattoso@brasmol.com.br</t>
+  </si>
+  <si>
+    <t>Auxiliar de Controle de Qualidade</t>
+  </si>
+  <si>
+    <t>Coordenador da Gestão de Qualidade</t>
+  </si>
+  <si>
+    <t>Almoxarife JR</t>
+  </si>
+  <si>
+    <t>Copeira</t>
+  </si>
+  <si>
+    <t>https://i.postimg.cc/KjHY8JXQ/Eduardo-Mattozo.jpg</t>
+  </si>
+  <si>
+    <t>Compradora JR</t>
+  </si>
+  <si>
+    <t>Analista Técnico de Desenvolvimento</t>
+  </si>
+  <si>
+    <t>Inspetor de Qualidade Senior</t>
+  </si>
+  <si>
+    <t>linkedin</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/dealmeidasilva/</t>
+  </si>
+  <si>
+    <t>descricao</t>
+  </si>
+  <si>
+    <t>Profissional com mais de 15 anos de experiência na área de tecnologia da informação, atuando principalmente como Supervisor de TI. Com uma sólida formação em Redes de Computadores e atualmente cursando Engenharia da Computação, possui vasta experiência em gestão de equipes, implementação de infraestrutura de TI e automação de processos.
+Ao longo da sua carreira, se destacou por liderar projetos de transformação digital, redução de custos e melhoria contínua, sempre com foco em inovação e eficiência operacional.
+Atualmente, está aprofundando seus conhecimentos em metodologias ágeis e frameworks como Scrum e Kanban, com o objetivo de aprimorar ainda mais suas habilidades em gestão de projetos e processos.</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/goveia-lacerda-03637248/</t>
+  </si>
+  <si>
+    <t>Profissional com mais de 15 anos de experiência na área de gestão da qualidade, tendo recentemente atuando como Coordenador do Sistema de Gestão da Qualidade. Com formação em Tecnologia de Gestão da Qualidade, possui uma sólida experiência na implementação de sistemas de qualidade baseados nas normas ISO 9001 e IATF 16949, garantindo a conformidade e a excelência nos processos produtivos.
+Ao longo de sua carreira, destacou-se por liderar projetos de homologação e qualificação de fornecedores, mapeamento de processos, e controle de indicadores de desempenho de qualidade, sempre focado em alcançar melhorias contínuas e satisfação dos clientes.
+Atualmente, está à frente do sistema de gestão da qualidade da empresa, onde lidera auditorias internas e externas, além de promover a capacitação da equipe para manter altos padrões de qualidade. Seu foco contínuo está na implementação de melhorias nos processos operacionais e na inovação das ferramentas de controle de qualidade.</t>
+  </si>
+  <si>
+    <t>É uma profissional com vasta experiência na área de produção industrial, tendo recentemente sido promovido do setor de Acabamento para o Controle de Qualidade, onde tem desempenhado um papel crucial na melhoria dos processos de controle de qualidade.
+Formado em Metrologia pelo SENAI, Aiume possui habilidades sólidas no manuseio de instrumentos de medição de alta precisão, como paquímetros, micrômetros e relógios comparadores. Essa formação técnica é fundamental para garantir a qualidade dos produtos e a conformidade com as normas técnicas.
+Ao longo da sua carreira, tem se destacado pela atenção aos detalhes e pela capacidade de adaptação em novos desafios, com um foco contínuo em assegurar que todos os processos estejam dentro dos mais altos padrões de qualidade.
+Atualmente, ele está se aprofundando em metodologias de controle de qualidade e ferramentas de medição avançada, trazendo inovação e excelência para a empresa.</t>
+  </si>
+  <si>
+    <t>Profissional com mais de 5 anos de experiência em setores operacionais, com uma sólida trajetória que abrange cargos de Atendente, Auxiliar Geral e, mais recentemente, Almoxarife Jr. Após atuar no setor de Expedição, onde desenvolveu habilidades logísticas e operacionais, Christopher foi promovido para o Almoxarifado, assumindo responsabilidades mais complexas na organização e controle de estoque.
+Atualmente, está se aprofundando nas rotinas do almoxarifado, onde utiliza suas competências em controle de estoque para garantir a disponibilidade e organização dos materiais.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -418,6 +456,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -444,9 +490,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -762,10 +827,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C900014C-14C8-4838-8849-A03641E53F4B}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,49 +840,60 @@
     <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="62.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="52.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="88.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" t="s">
         <v>99</v>
       </c>
-      <c r="C1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D1" t="s">
-        <v>101</v>
-      </c>
-      <c r="E1" t="s">
-        <v>102</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="225" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>145</v>
       </c>
-      <c r="C2" t="s">
-        <v>95</v>
-      </c>
-      <c r="D2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -837,49 +913,58 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:8" s="6" customFormat="1" ht="210" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="6">
         <v>137</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="3" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" s="3">
+        <v>132</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5">
-        <v>132</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H5" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>140</v>
@@ -888,330 +973,334 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B7">
         <v>117</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D7" t="s">
-        <v>108</v>
+        <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8">
         <v>115</v>
       </c>
       <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B9">
         <v>126</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>127</v>
       </c>
       <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11">
         <v>115</v>
       </c>
       <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="1" t="s">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>32</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>34</v>
       </c>
       <c r="B12">
         <v>141</v>
       </c>
       <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D12" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>39</v>
       </c>
       <c r="B13">
         <v>154</v>
       </c>
       <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B14">
         <v>120</v>
       </c>
       <c r="C14" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D14" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B15">
         <v>113</v>
       </c>
       <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>49</v>
       </c>
       <c r="B16">
         <v>128</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B17">
         <v>121</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D17" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B18">
         <v>111</v>
       </c>
       <c r="C18" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D18" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F18" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B19">
         <v>131</v>
       </c>
       <c r="C19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>59</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>62</v>
       </c>
       <c r="B20">
         <v>114</v>
       </c>
       <c r="C20" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" t="s">
+        <v>61</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D20" t="s">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>64</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>67</v>
       </c>
       <c r="B21">
         <v>135</v>
       </c>
       <c r="C21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D21" t="s">
-        <v>56</v>
+        <v>121</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B22">
         <v>117</v>
       </c>
       <c r="C22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D22" t="s">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>72</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>75</v>
       </c>
       <c r="B23">
         <v>118</v>
@@ -1220,104 +1309,110 @@
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" s="3" customFormat="1" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" s="3">
+        <v>139</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B24">
-        <v>139</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="F24" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D24" t="s">
+      <c r="G24" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>87</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>90</v>
       </c>
       <c r="B25">
         <v>147</v>
       </c>
       <c r="C25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D25" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B26">
         <v>130</v>
       </c>
       <c r="C26" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B27">
         <v>111</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D27" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B28">
         <v>145</v>
       </c>
       <c r="C28" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D28" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1376,6 +1471,9 @@
     <hyperlink ref="E14" r:id="rId47" xr:uid="{DDA1AF5D-ACDF-433A-8BD3-4D814E2618E0}"/>
     <hyperlink ref="E9" r:id="rId48" xr:uid="{91A7B212-F61A-4001-8B0E-4D95918FCF47}"/>
     <hyperlink ref="F9" r:id="rId49" xr:uid="{487A1BAA-2AB3-44FE-B188-20C6D73F4F34}"/>
+    <hyperlink ref="F14" r:id="rId50" xr:uid="{8DAD4A55-75BE-4828-8D8B-D161768AF528}"/>
+    <hyperlink ref="G24" r:id="rId51" xr:uid="{F2C9DC16-5A15-40AB-AEB3-E617128F4E75}"/>
+    <hyperlink ref="G4" r:id="rId52" xr:uid="{4F1ACAF8-C7AB-4BB6-A462-96C6CB5B23DD}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>